<commit_message>
Organizing reports, text, and other functionalities.
</commit_message>
<xml_diff>
--- a/inst/app/template/template_terneiraTrack.xlsx
+++ b/inst/app/template/template_terneiraTrack.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tadeuederdasilva/Documents/Postdoc - UVM/terneiraTrack/inst/app/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94CAF33-657A-444F-B371-2150EA9D6E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA4884A-D565-2C40-B186-0D2432E38A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16900" xr2:uid="{AA3DFA79-351B-6E48-827C-213E71C95748}"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16900" activeTab="2" xr2:uid="{AA3DFA79-351B-6E48-827C-213E71C95748}"/>
   </bookViews>
   <sheets>
     <sheet name="1- cadastro" sheetId="1" r:id="rId1"/>
     <sheet name="2- crescimento" sheetId="2" r:id="rId2"/>
+    <sheet name="3- saúde" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,12 +38,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Nome da fazenda</t>
   </si>
   <si>
     <t>Proprietario</t>
+  </si>
+  <si>
+    <t>Num. Bezerra</t>
+  </si>
+  <si>
+    <t>Data nasc.</t>
+  </si>
+  <si>
+    <t>Peso Nasc. (kg)</t>
+  </si>
+  <si>
+    <t>Data Pesagem</t>
+  </si>
+  <si>
+    <t>Peso (kg)</t>
+  </si>
+  <si>
+    <t>Data Tratamento</t>
+  </si>
+  <si>
+    <t>Tratmento</t>
+  </si>
+  <si>
+    <t>Doença</t>
+  </si>
+  <si>
+    <t>Obs.</t>
   </si>
 </sst>
 </file>
@@ -78,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3BCAE-6FE3-5347-AA17-7BBA0C364195}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -437,23 +466,168 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4463A2-7D4A-0F4A-AA75-4377C5A07881}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45394</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1">
+        <f>B2+30</f>
+        <v>45424</v>
+      </c>
+      <c r="E2">
+        <f>C2+30*0.5</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45395</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D6" si="0">B3+30</f>
+        <v>45425</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="1">C3+30*0.5</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45396</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>45426</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45397</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>45427</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45398</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>45428</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60130C9-29B9-7840-96ED-52B4D21B54FE}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Developing the growth model.
</commit_message>
<xml_diff>
--- a/inst/app/template/template_terneiraTrack.xlsx
+++ b/inst/app/template/template_terneiraTrack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tadeuederdasilva/Documents/Postdoc - UVM/terneiraTrack/inst/app/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA4884A-D565-2C40-B186-0D2432E38A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3063CD-4818-3041-B7B7-3B3EC7524D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16900" activeTab="2" xr2:uid="{AA3DFA79-351B-6E48-827C-213E71C95748}"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16900" activeTab="1" xr2:uid="{AA3DFA79-351B-6E48-827C-213E71C95748}"/>
   </bookViews>
   <sheets>
     <sheet name="1- cadastro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Nome da fazenda</t>
   </si>
@@ -71,6 +71,33 @@
   </si>
   <si>
     <t>Obs.</t>
+  </si>
+  <si>
+    <t>Localidade</t>
+  </si>
+  <si>
+    <t>Técnico Resp.</t>
+  </si>
+  <si>
+    <t>São José</t>
+  </si>
+  <si>
+    <t>Tadeu Silva</t>
+  </si>
+  <si>
+    <t>Carvalhos-MG</t>
+  </si>
+  <si>
+    <t>Desmamada</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Idade ao Desm.</t>
+  </si>
+  <si>
+    <t>Sim</t>
   </si>
 </sst>
 </file>
@@ -106,9 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,20 +471,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3BCAE-6FE3-5347-AA17-7BBA0C364195}">
-  <dimension ref="A1:B1"/>
+  <sheetPr>
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" hidden="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -466,19 +524,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4463A2-7D4A-0F4A-AA75-4377C5A07881}">
-  <dimension ref="A1:E7"/>
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -494,8 +562,14 @@
       <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -506,15 +580,16 @@
         <v>35</v>
       </c>
       <c r="D2" s="1">
-        <f>B2+30</f>
         <v>45424</v>
       </c>
-      <c r="E2">
-        <f>C2+30*0.5</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="2">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -525,15 +600,16 @@
         <v>32</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D6" si="0">B3+30</f>
         <v>45425</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E6" si="1">C3+30*0.5</f>
+      <c r="E3" s="2">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -544,15 +620,16 @@
         <v>40</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
         <v>45426</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>52</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -563,15 +640,16 @@
         <v>42</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
         <v>45427</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -582,16 +660,262 @@
         <v>40</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
         <v>45428</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
+      <c r="E6" s="2">
+        <v>46</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45399</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45429</v>
+      </c>
+      <c r="E7" s="2">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45400</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45430</v>
+      </c>
+      <c r="E8" s="2">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45401</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45431</v>
+      </c>
+      <c r="E9" s="2">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45402</v>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45432</v>
+      </c>
+      <c r="E10" s="2">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45403</v>
+      </c>
+      <c r="C11">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45433</v>
+      </c>
+      <c r="E11" s="2">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45404</v>
+      </c>
+      <c r="C12">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45434</v>
+      </c>
+      <c r="E12" s="2">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45405</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45435</v>
+      </c>
+      <c r="E13" s="2">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45406</v>
+      </c>
+      <c r="C14">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45436</v>
+      </c>
+      <c r="E14" s="2">
+        <v>55</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45407</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>45437</v>
+      </c>
+      <c r="E15" s="2">
+        <v>45</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45408</v>
+      </c>
+      <c r="C16">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1">
+        <v>45438</v>
+      </c>
+      <c r="E16" s="2">
+        <v>61</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45352</v>
+      </c>
+      <c r="C17">
+        <v>44</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45448</v>
+      </c>
+      <c r="E17">
+        <f>C17+90*0.85</f>
+        <v>120.5</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45353</v>
+      </c>
+      <c r="C18">
+        <v>45</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45449</v>
+      </c>
+      <c r="E18">
+        <f>C18+90*0.85</f>
+        <v>121.5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -600,10 +924,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60130C9-29B9-7840-96ED-52B4D21B54FE}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adjustments in the calf growth module.
</commit_message>
<xml_diff>
--- a/inst/app/template/template_terneiraTrack.xlsx
+++ b/inst/app/template/template_terneiraTrack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tadeuederdasilva/Documents/Postdoc - UVM/terneiraTrack/inst/app/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3063CD-4818-3041-B7B7-3B3EC7524D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A9A843-1D51-E746-8887-78D7165E2105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16900" activeTab="1" xr2:uid="{AA3DFA79-351B-6E48-827C-213E71C95748}"/>
   </bookViews>
@@ -37,6 +37,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2D855A95-58D7-3343-B7EF-F257A8111E89}</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2D855A95-58D7-3343-B7EF-F257A8111E89}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Caso a bezerra não tenha sido desaleitada, deixe vazio, ou seja, não adicione nenhum texto à célula.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
@@ -49,9 +67,6 @@
     <t>Num. Bezerra</t>
   </si>
   <si>
-    <t>Data nasc.</t>
-  </si>
-  <si>
     <t>Peso Nasc. (kg)</t>
   </si>
   <si>
@@ -91,13 +106,16 @@
     <t>Desmamada</t>
   </si>
   <si>
-    <t>Não</t>
-  </si>
-  <si>
     <t>Idade ao Desm.</t>
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Nao</t>
+  </si>
+  <si>
+    <t>Data Nasc.</t>
   </si>
 </sst>
 </file>
@@ -152,6 +170,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Tadeu Da Silva" id="{41129B21-193A-814D-AC63-FBA13585EE41}" userId="S::tdasilva@uvm.edu::6a44bf9a-f526-4216-96c9-1325078cd530" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,6 +493,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2024-12-04T19:43:44.84" personId="{41129B21-193A-814D-AC63-FBA13585EE41}" id="{2D855A95-58D7-3343-B7EF-F257A8111E89}">
+    <text>Caso a bezerra não tenha sido desaleitada, deixe vazio, ou seja, não adicione nenhum texto à célula.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3BCAE-6FE3-5347-AA17-7BBA0C364195}">
   <sheetPr>
@@ -497,24 +529,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -523,15 +555,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4463A2-7D4A-0F4A-AA75-4377C5A07881}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4463A2-7D4A-0F4A-AA75-4377C5A07881}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,22 +583,22 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
       <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -586,7 +618,7 @@
         <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -606,7 +638,7 @@
         <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -626,7 +658,7 @@
         <v>52</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -646,7 +678,7 @@
         <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -666,7 +698,7 @@
         <v>46</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -686,7 +718,7 @@
         <v>50</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -706,7 +738,7 @@
         <v>55</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -726,7 +758,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -746,7 +778,7 @@
         <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -766,7 +798,7 @@
         <v>55</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -786,7 +818,7 @@
         <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -806,7 +838,7 @@
         <v>48</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -826,7 +858,7 @@
         <v>55</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -846,7 +878,7 @@
         <v>45</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -866,7 +898,7 @@
         <v>61</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -887,7 +919,7 @@
         <v>120.5</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G17">
         <v>96</v>
@@ -911,14 +943,53 @@
         <v>121.5</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G18">
         <v>97</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F18" xr:uid="{F449A7E1-7042-DD49-8313-8365B1D935B2}">
+      <formula1>"Sim, Nao"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28" xr:uid="{A715C9BE-B546-0847-8714-422DBB87E148}">
+      <formula1>"Sim, Nao, Vazio"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -945,16 +1016,16 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>